<commit_message>
"Updated grades and images for week 10."
</commit_message>
<xml_diff>
--- a/_files/student_grades_g1.xlsx
+++ b/_files/student_grades_g1.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="121">
   <si>
     <t>firstName</t>
   </si>
@@ -389,6 +389,12 @@
   </si>
   <si>
     <t>&lt;span&gt;Guía #7 - &lt;/span&gt;   Taller de fin de perido 2</t>
+  </si>
+  <si>
+    <t>Jeisson debes recordar restar al vecino que te prestó, ya que este número no queda igual.</t>
+  </si>
+  <si>
+    <t>Sofi cuando prestas con el vecino el número al que le prestan no siempre se convierte en 10, eso depende del número que tengas en las unidades.</t>
   </si>
 </sst>
 </file>
@@ -438,7 +444,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -523,12 +529,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -557,7 +557,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -642,15 +642,6 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
@@ -658,9 +649,6 @@
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -991,7 +979,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="3" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="T28" sqref="T28"/>
+      <selection pane="topRight" activeCell="U29" sqref="U29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,7 +1068,7 @@
       </c>
       <c r="B2" s="14">
         <f ca="1">TODAY()</f>
-        <v>43974</v>
+        <v>43981</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>93</v>
@@ -1198,8 +1186,12 @@
       <c r="S3" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="T3" s="35"/>
-      <c r="U3" s="5"/>
+      <c r="T3" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="4" spans="1:21" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -1312,11 +1304,19 @@
       <c r="O5" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="P5" s="27"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="32"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="34"/>
+      <c r="P5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="R5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="T5" s="31"/>
       <c r="U5" s="5"/>
     </row>
     <row r="6" spans="1:21" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -1371,10 +1371,18 @@
       <c r="Q6" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="R6" s="31"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="35"/>
-      <c r="U6" s="5"/>
+      <c r="R6" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="T6" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="U6" s="5" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="7" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
@@ -1499,8 +1507,12 @@
       <c r="S8" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="T8" s="35"/>
-      <c r="U8" s="5"/>
+      <c r="T8" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="U8" s="5" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="9" spans="1:21" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
@@ -1560,8 +1572,12 @@
       <c r="S9" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="T9" s="35"/>
-      <c r="U9" s="5"/>
+      <c r="T9" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="U9" s="5" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="10" spans="1:21" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
@@ -1621,8 +1637,12 @@
       <c r="S10" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="T10" s="35"/>
-      <c r="U10" s="5"/>
+      <c r="T10" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="U10" s="5" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="11" spans="1:21" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
@@ -1877,8 +1897,12 @@
       <c r="S14" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="T14" s="35"/>
-      <c r="U14" s="5"/>
+      <c r="T14" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="U14" s="5" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="15" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
@@ -1938,8 +1962,12 @@
       <c r="S15" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="T15" s="35"/>
-      <c r="U15" s="15"/>
+      <c r="T15" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="U15" s="15" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
@@ -2058,10 +2086,18 @@
       <c r="Q17" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="R17" s="30"/>
-      <c r="S17" s="15"/>
-      <c r="T17" s="35"/>
-      <c r="U17" s="15"/>
+      <c r="R17" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="S17" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="T17" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="U17" s="15" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="18" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
@@ -2245,10 +2281,18 @@
       <c r="Q20" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="R20" s="36"/>
-      <c r="S20" s="15"/>
-      <c r="T20" s="35"/>
-      <c r="U20" s="15"/>
+      <c r="R20" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="S20" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="T20" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="U20" s="15" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
@@ -2290,9 +2334,9 @@
       <c r="O21" s="15"/>
       <c r="P21" s="27"/>
       <c r="Q21" s="15"/>
-      <c r="R21" s="33"/>
+      <c r="R21" s="30"/>
       <c r="S21" s="15"/>
-      <c r="T21" s="34"/>
+      <c r="T21" s="31"/>
       <c r="U21" s="15"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
@@ -2353,8 +2397,12 @@
       <c r="S22" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="T22" s="35"/>
-      <c r="U22" s="15"/>
+      <c r="T22" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="U22" s="15" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
@@ -2402,9 +2450,9 @@
       <c r="O23" s="15"/>
       <c r="P23" s="27"/>
       <c r="Q23" s="15"/>
-      <c r="R23" s="33"/>
+      <c r="R23" s="30"/>
       <c r="S23" s="15"/>
-      <c r="T23" s="34"/>
+      <c r="T23" s="31"/>
       <c r="U23" s="15"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
@@ -2465,8 +2513,12 @@
       <c r="S24" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="T24" s="35"/>
-      <c r="U24" s="15"/>
+      <c r="T24" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="U24" s="15" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
@@ -2526,7 +2578,7 @@
       <c r="S25" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="T25" s="35"/>
+      <c r="T25" s="32"/>
       <c r="U25" s="15"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
@@ -2652,8 +2704,12 @@
       <c r="S27" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="T27" s="35"/>
-      <c r="U27" s="15"/>
+      <c r="T27" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="U27" s="15" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
@@ -2778,8 +2834,12 @@
       <c r="S29" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="T29" s="35"/>
-      <c r="U29" s="15"/>
+      <c r="T29" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="U29" s="15" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="36" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated images for week #11. Grade platform now with information about exam.
</commit_message>
<xml_diff>
--- a/_files/student_grades_g1.xlsx
+++ b/_files/student_grades_g1.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="125">
   <si>
     <t>firstName</t>
   </si>
@@ -395,6 +395,18 @@
   </si>
   <si>
     <t>Sofi cuando prestas con el vecino el número al que le prestan no siempre se convierte en 10, eso depende del número que tengas en las unidades.</t>
+  </si>
+  <si>
+    <t>&lt;span&gt;Examen - &lt;/span&gt;   fin de periodo 2</t>
+  </si>
+  <si>
+    <t>¡Excelente!</t>
+  </si>
+  <si>
+    <t>4.3</t>
+  </si>
+  <si>
+    <t>¡Muy bien!</t>
   </si>
 </sst>
 </file>
@@ -648,7 +660,7 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -975,11 +987,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U49"/>
+  <dimension ref="A1:W49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U29" sqref="U29"/>
+      <pane xSplit="3" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W24" sqref="W24:W25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -995,9 +1007,11 @@
     <col min="19" max="19" width="13.28515625" customWidth="1"/>
     <col min="20" max="20" width="12.7109375" customWidth="1"/>
     <col min="21" max="21" width="13.28515625" customWidth="1"/>
+    <col min="22" max="22" width="12.7109375" customWidth="1"/>
+    <col min="23" max="23" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="61.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="61.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>5</v>
       </c>
@@ -1061,14 +1075,20 @@
       <c r="U1" s="6" t="s">
         <v>8</v>
       </c>
+      <c r="V1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:21" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="14">
         <f ca="1">TODAY()</f>
-        <v>43981</v>
+        <v>43989</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>93</v>
@@ -1127,8 +1147,14 @@
       <c r="U2" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="V2" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:21" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>12</v>
       </c>
@@ -1192,8 +1218,14 @@
       <c r="U3" s="5" t="s">
         <v>97</v>
       </c>
+      <c r="V3" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="4" spans="1:21" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>13</v>
       </c>
@@ -1257,8 +1289,14 @@
       <c r="U4" s="5" t="s">
         <v>112</v>
       </c>
+      <c r="V4" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="W4" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="5" spans="1:21" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>14</v>
       </c>
@@ -1316,10 +1354,20 @@
       <c r="S5" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="T5" s="31"/>
-      <c r="U5" s="5"/>
+      <c r="T5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="U5" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="V5" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="W5" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="6" spans="1:21" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>15</v>
       </c>
@@ -1383,8 +1431,14 @@
       <c r="U6" s="5" t="s">
         <v>99</v>
       </c>
+      <c r="V6" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="W6" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="7" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>16</v>
       </c>
@@ -1448,8 +1502,14 @@
       <c r="U7" s="5" t="s">
         <v>96</v>
       </c>
+      <c r="V7" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="W7" s="5" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="8" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>17</v>
       </c>
@@ -1513,8 +1573,14 @@
       <c r="U8" s="5" t="s">
         <v>96</v>
       </c>
+      <c r="V8" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="W8" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="9" spans="1:21" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>18</v>
       </c>
@@ -1578,8 +1644,14 @@
       <c r="U9" s="5" t="s">
         <v>96</v>
       </c>
+      <c r="V9" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="W9" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="10" spans="1:21" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>19</v>
       </c>
@@ -1643,8 +1715,14 @@
       <c r="U10" s="5" t="s">
         <v>97</v>
       </c>
+      <c r="V10" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="W10" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="11" spans="1:21" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>20</v>
       </c>
@@ -1708,8 +1786,14 @@
       <c r="U11" s="5" t="s">
         <v>96</v>
       </c>
+      <c r="V11" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="W11" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="12" spans="1:21" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>21</v>
       </c>
@@ -1773,8 +1857,14 @@
       <c r="U12" s="5" t="s">
         <v>95</v>
       </c>
+      <c r="V12" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="W12" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="13" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>22</v>
       </c>
@@ -1838,8 +1928,14 @@
       <c r="U13" s="5" t="s">
         <v>114</v>
       </c>
+      <c r="V13" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="W13" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>23</v>
       </c>
@@ -1903,8 +1999,14 @@
       <c r="U14" s="5" t="s">
         <v>99</v>
       </c>
+      <c r="V14" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="W14" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="15" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>24</v>
       </c>
@@ -1968,8 +2070,14 @@
       <c r="U15" s="15" t="s">
         <v>96</v>
       </c>
+      <c r="V15" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="W15" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>25</v>
       </c>
@@ -2033,8 +2141,14 @@
       <c r="U16" s="15" t="s">
         <v>96</v>
       </c>
+      <c r="V16" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="W16" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="17" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>26</v>
       </c>
@@ -2098,8 +2212,14 @@
       <c r="U17" s="15" t="s">
         <v>119</v>
       </c>
+      <c r="V17" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="W17" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="18" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>27</v>
       </c>
@@ -2163,8 +2283,14 @@
       <c r="U18" s="15" t="s">
         <v>116</v>
       </c>
+      <c r="V18" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="W18" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>28</v>
       </c>
@@ -2228,8 +2354,14 @@
       <c r="U19" s="15" t="s">
         <v>115</v>
       </c>
+      <c r="V19" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="W19" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>29</v>
       </c>
@@ -2293,8 +2425,14 @@
       <c r="U20" s="15" t="s">
         <v>120</v>
       </c>
+      <c r="V20" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="W20" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>30</v>
       </c>
@@ -2338,8 +2476,14 @@
       <c r="S21" s="15"/>
       <c r="T21" s="31"/>
       <c r="U21" s="15"/>
+      <c r="V21" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="W21" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>31</v>
       </c>
@@ -2403,8 +2547,14 @@
       <c r="U22" s="15" t="s">
         <v>97</v>
       </c>
+      <c r="V22" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="W22" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>32</v>
       </c>
@@ -2454,8 +2604,10 @@
       <c r="S23" s="15"/>
       <c r="T23" s="31"/>
       <c r="U23" s="15"/>
+      <c r="V23" s="31"/>
+      <c r="W23" s="15"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>33</v>
       </c>
@@ -2519,8 +2671,14 @@
       <c r="U24" s="15" t="s">
         <v>96</v>
       </c>
+      <c r="V24" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="W24" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>34</v>
       </c>
@@ -2578,10 +2736,18 @@
       <c r="S25" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="T25" s="32"/>
+      <c r="T25" s="26" t="s">
+        <v>3</v>
+      </c>
       <c r="U25" s="15"/>
+      <c r="V25" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="W25" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>35</v>
       </c>
@@ -2645,8 +2811,14 @@
       <c r="U26" s="15" t="s">
         <v>100</v>
       </c>
+      <c r="V26" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="W26" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>36</v>
       </c>
@@ -2710,8 +2882,14 @@
       <c r="U27" s="15" t="s">
         <v>95</v>
       </c>
+      <c r="V27" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="W27" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>37</v>
       </c>
@@ -2775,8 +2953,14 @@
       <c r="U28" s="15" t="s">
         <v>98</v>
       </c>
+      <c r="V28" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="W28" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>38</v>
       </c>
@@ -2839,6 +3023,12 @@
       </c>
       <c r="U29" s="15" t="s">
         <v>96</v>
+      </c>
+      <c r="V29" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="W29" s="5" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>